<commit_message>
Updated Keyless Script, and Relationship Table.
</commit_message>
<xml_diff>
--- a/ZBabcock_RelationshipTable.xlsx
+++ b/ZBabcock_RelationshipTable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="28">
   <si>
     <t>ActivityTypes</t>
   </si>
@@ -88,13 +88,28 @@
   </si>
   <si>
     <t>Afterwards, if an inserted BusinessType doesn't exist in BusinessTypes, raise error and rollback.</t>
+  </si>
+  <si>
+    <t>NDR</t>
+  </si>
+  <si>
+    <t>X = Does not Exist</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>' = Relationship, but not covered by trigger</t>
+  </si>
+  <si>
+    <t>info needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,19 +124,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,7 +170,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -470,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,9 +520,9 @@
     <col min="11" max="11" width="22.28515625" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" customWidth="1"/>
     <col min="17" max="17" width="30.28515625" customWidth="1"/>
     <col min="18" max="18" width="24" customWidth="1"/>
     <col min="19" max="19" width="24.42578125" customWidth="1"/>
@@ -608,9 +637,15 @@
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
@@ -620,23 +655,47 @@
       <c r="G4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
+      <c r="T4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -710,9 +769,15 @@
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
@@ -722,9 +787,15 @@
       <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="H6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="K6" s="3" t="s">
         <v>22</v>
       </c>
@@ -735,9 +806,15 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
+      <c r="Q6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
@@ -746,9 +823,15 @@
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
@@ -768,8 +851,12 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="N7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3" t="s">
         <v>17</v>
@@ -786,9 +873,15 @@
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
@@ -828,7 +921,9 @@
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
@@ -846,7 +941,9 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="P9" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="3" t="s">
         <v>16</v>
@@ -860,9 +957,15 @@
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
@@ -895,6 +998,16 @@
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>